<commit_message>
updated accuracy with unknowns included
</commit_message>
<xml_diff>
--- a/Predictions_QWEN0.5B/wave1_all_predictionsFINAL/prefinetuned_predictions_imputed_w1.xlsx
+++ b/Predictions_QWEN0.5B/wave1_all_predictionsFINAL/prefinetuned_predictions_imputed_w1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PhD_Yearwise_Materials\PhD Year 3 Materials\NLPOR 2025\LLM-NLPOR-Work\Predictions_QWEN0.5B\wave1_all_predictionsFINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD4A4FE-6F94-420F-9E34-A9A2902201FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DCD2D7-77DC-4F07-8E12-E7527649CE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9220,10 +9220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2146"/>
+  <dimension ref="A1:O2146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9235,7 +9235,7 @@
     <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9243,7 +9243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -9369,7 +9369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -9380,7 +9380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -9428,7 +9428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -9436,7 +9436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -9510,7 +9510,7 @@
         <v>1721.5090909090909</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -9555,6 +9555,10 @@
       <c r="M16">
         <f>(M13-M14)/(J16-M14)</f>
         <v>-3.5634552636098034E-3</v>
+      </c>
+      <c r="O16">
+        <f>1720/2145</f>
+        <v>0.80186480186480191</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>